<commit_message>
dei fix no que tinha errado
</commit_message>
<xml_diff>
--- a/src/excels/meningeal/updates/merged_top_genes.xlsx
+++ b/src/excels/meningeal/updates/merged_top_genes.xlsx
@@ -7,30 +7,31 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="MeV.Vascular.0" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="MeV.Endothelial.0" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="MeV.1.4.11" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="MeV.1.4.13" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="MeV.1.4.15" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="MeV.1.4.2" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="MeV.1.4.20" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="MeV.1.4.21" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet name="MeV.1.4.4" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet name="MeV.Vascular.2" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet name="MeV.1.4.6" sheetId="10" state="visible" r:id="rId10"/>
-    <sheet name="MeV.1.4.7" sheetId="11" state="visible" r:id="rId11"/>
-    <sheet name="MeV.1.4.8" sheetId="12" state="visible" r:id="rId12"/>
-    <sheet name="MeV.2.1" sheetId="13" state="visible" r:id="rId13"/>
-    <sheet name="MeV.2.8" sheetId="14" state="visible" r:id="rId14"/>
-    <sheet name="MeV.3.17" sheetId="15" state="visible" r:id="rId15"/>
-    <sheet name="MeV.Proliferative_Fibr.0" sheetId="16" state="visible" r:id="rId16"/>
-    <sheet name="MeV.Pericytes.0" sheetId="17" state="visible" r:id="rId17"/>
-    <sheet name="MeV.4.12" sheetId="18" state="visible" r:id="rId18"/>
-    <sheet name="MeV.Vascular.1" sheetId="19" state="visible" r:id="rId19"/>
-    <sheet name="MeV.4.26" sheetId="20" state="visible" r:id="rId20"/>
-    <sheet name="MeV.4.30" sheetId="21" state="visible" r:id="rId21"/>
-    <sheet name="MeV.SMC.0" sheetId="22" state="visible" r:id="rId22"/>
-    <sheet name="MeV.4.34" sheetId="23" state="visible" r:id="rId23"/>
-    <sheet name="MeV.4.4" sheetId="24" state="visible" r:id="rId24"/>
+    <sheet name="MeV.1.4.12" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="MeV.1.4.13" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="MeV.Endothelial.3" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="MeV.1.4.2" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="MeV.Endothelial_Injury.4" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="MeV.Immune_doublets.0" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="MeV.1.4.4" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="MeV.Endothelial.2" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="MeV.1.4.6" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet name="MeV.1.4.7" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet name="MeV.Low_Quality.0" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet name="MeV.2.1" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet name="MeV.2.8" sheetId="15" state="visible" r:id="rId15"/>
+    <sheet name="MeV.3.17" sheetId="16" state="visible" r:id="rId16"/>
+    <sheet name="MeV.Proliferative_Fibr.0" sheetId="17" state="visible" r:id="rId17"/>
+    <sheet name="MeV.Pericytes.0" sheetId="18" state="visible" r:id="rId18"/>
+    <sheet name="MeV.VLMC.1" sheetId="19" state="visible" r:id="rId19"/>
+    <sheet name="MeV.Endothelial.1" sheetId="20" state="visible" r:id="rId20"/>
+    <sheet name="MeV.Epithelial_ECad.0" sheetId="21" state="visible" r:id="rId21"/>
+    <sheet name="MeV.Fib_CD34.0" sheetId="22" state="visible" r:id="rId22"/>
+    <sheet name="MeV.SMC.0" sheetId="23" state="visible" r:id="rId23"/>
+    <sheet name="MeV.4.34" sheetId="24" state="visible" r:id="rId24"/>
+    <sheet name="MeV.VLMC.0" sheetId="25" state="visible" r:id="rId25"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -574,7 +575,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -602,11 +603,11 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Trpm3</t>
+          <t>Slco1c1</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.99</v>
+        <v>0.68</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -617,11 +618,11 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Il31ra</t>
+          <t>Slco1a4</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.7</v>
+        <v>0.95</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
@@ -632,11 +633,11 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Dcdc2a</t>
+          <t>Slc7a5</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.41</v>
+        <v>0.44</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
@@ -647,56 +648,56 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Cyp26b1</t>
+          <t>Tfrc</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.42</v>
+        <v>0.37</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>0.3, 0.4</t>
+          <t>0.3</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Scn7a</t>
+          <t>Nostrin</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.38</v>
+        <v>0.41</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>0.3</t>
+          <t>0.3, 0.4</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Col22a1</t>
+          <t>Prom1</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.61</v>
+        <v>0.43</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>0.4, 0.5</t>
+          <t>0.4</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Igf1</t>
+          <t>Spock2</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.86</v>
+        <v>0.66</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
@@ -707,13 +708,28 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Glis3</t>
+          <t>Lef1</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.71</v>
+        <v>0.86</v>
       </c>
       <c r="C9" t="inlineStr">
+        <is>
+          <t>0.5</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Slc39a10</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="C10" t="inlineStr">
         <is>
           <t>0.5</t>
         </is>
@@ -725,6 +741,147 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Gene</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>pts</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>pts of origin</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Trpm3</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>0.99</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>0.3, 0.4, 0.5</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Il31ra</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>0.3, 0.4, 0.5</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Dcdc2a</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>0.41</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>0.3, 0.4</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Cyp26b1</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>0.42</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>0.3, 0.4</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Col22a1</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>0.61</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>0.3, 0.4, 0.5</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Igf1</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>0.86</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>0.5</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Glis3</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>0.71</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>0.5</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -773,11 +930,11 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Pla1a</t>
+          <t>Igfbp3</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.31</v>
+        <v>0.3</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
@@ -788,11 +945,11 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Igfbp3</t>
+          <t>Pla1a</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.3</v>
+        <v>0.31</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
@@ -803,11 +960,11 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Slc7a11</t>
+          <t>Ranbp3l</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.86</v>
+        <v>0.89</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
@@ -818,11 +975,11 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Ranbp3l</t>
+          <t>Slc7a11</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.89</v>
+        <v>0.86</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
@@ -870,207 +1027,6 @@
         <v>0.9399999999999999</v>
       </c>
       <c r="C9" t="inlineStr">
-        <is>
-          <t>0.5</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C12"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Gene</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>pts</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>pts of origin</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Ftl1</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>0.38</v>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>0.3</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Rpl18a</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>0.4</v>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>0.3, 0.4</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Rpl19</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>0.37</v>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>0.3</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Rpl41</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>0.51</v>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>0.3, 0.4, 0.5</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Rpl26</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>0.39</v>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>0.3</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Rplp1</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>0.58</v>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>0.4, 0.5</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Rps23</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
-        <v>0.4</v>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>0.4</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>Fau</t>
-        </is>
-      </c>
-      <c r="B9" t="n">
-        <v>0.42</v>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>0.4</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Apoe</t>
-        </is>
-      </c>
-      <c r="B10" t="n">
-        <v>0.62</v>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>0.5</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>Tpt1</t>
-        </is>
-      </c>
-      <c r="B11" t="n">
-        <v>0.52</v>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>0.5</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>Tmsb4x</t>
-        </is>
-      </c>
-      <c r="B12" t="n">
-        <v>0.65</v>
-      </c>
-      <c r="C12" t="inlineStr">
         <is>
           <t>0.5</t>
         </is>
@@ -1115,131 +1071,131 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Ccbe1</t>
+          <t>Ftl1</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.49</v>
+        <v>0.38</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>0.3, 0.4</t>
+          <t>0.3</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Grem2</t>
+          <t>Rpl18a</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.35</v>
+        <v>0.4</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>0.3</t>
+          <t>0.3, 0.4</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Slc7a11</t>
+          <t>Rpl19</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.92</v>
+        <v>0.37</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>0.3, 0.4, 0.5</t>
+          <t>0.3</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Aox3</t>
+          <t>Rpl41</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.37</v>
+        <v>0.51</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>0.3</t>
+          <t>0.3, 0.4, 0.5</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Tmem132c</t>
+          <t>Rps23</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.34</v>
+        <v>0.4</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>0.3</t>
+          <t>0.3, 0.4</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Lama1</t>
+          <t>Rplp1</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.43</v>
+        <v>0.58</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>0.4</t>
+          <t>0.4, 0.5</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Col4a6</t>
+          <t>Fau</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.54</v>
+        <v>0.42</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>0.4, 0.5</t>
+          <t>0.4</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Ltbp1</t>
+          <t>Apoe</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.6</v>
+        <v>0.62</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>0.4, 0.5</t>
+          <t>0.5</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Slc1a3</t>
+          <t>Tpt1</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.59</v>
+        <v>0.52</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
@@ -1250,11 +1206,11 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Mrvi1</t>
+          <t>Tmsb4x</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.59</v>
+        <v>0.65</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
@@ -1268,6 +1224,192 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Gene</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>pts</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>pts of origin</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Ccbe1</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>0.49</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>0.3, 0.4</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Slc7a11</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>0.92</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>0.3, 0.4, 0.5</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Grem2</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>0.35</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>0.3</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Aox3</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>0.37</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>0.3</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Tmem132c</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>0.34</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>0.3</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Lama1</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>0.43</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>0.4</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Col4a6</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>0.54</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>0.4, 0.5</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Ltbp1</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>0.4, 0.5</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Mrvi1</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>0.59</v>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>0.5</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Igf1</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>0.76</v>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>0.5</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1393,7 +1535,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1534,7 +1676,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1613,11 +1755,11 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Tpx2</t>
+          <t>Knl1</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.62</v>
+        <v>0.67</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
@@ -1628,11 +1770,11 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Knl1</t>
+          <t>Hmmr</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.67</v>
+        <v>0.52</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
@@ -1645,7 +1787,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1761,162 +1903,6 @@
         <v>0.8100000000000001</v>
       </c>
       <c r="C7" t="inlineStr">
-        <is>
-          <t>0.4, 0.5</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Gene</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>pts</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>pts of origin</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Myoc</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>0.33</v>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>0.3</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Gm973</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>0.38</v>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>0.3</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Prps2</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>0.39</v>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>0.3</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Slc47a1</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>0.99</v>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>0.3, 0.4, 0.5</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Tbx15</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>0.61</v>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>0.3, 0.4, 0.5</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Tspan11</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>0.85</v>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>0.4, 0.5</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Slc4a10</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
-        <v>1</v>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>0.4, 0.5</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>Slc47a2</t>
-        </is>
-      </c>
-      <c r="B9" t="n">
-        <v>0.71</v>
-      </c>
-      <c r="C9" t="inlineStr">
         <is>
           <t>0.4, 0.5</t>
         </is>
@@ -1961,11 +1947,11 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Sema3g</t>
+          <t>Myoc</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.36</v>
+        <v>0.33</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -1976,26 +1962,26 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Bmx</t>
+          <t>Gm973</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.65</v>
+        <v>0.38</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>0.3, 0.4, 0.5</t>
+          <t>0.3</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Nos1</t>
+          <t>Prps2</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.36</v>
+        <v>0.39</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
@@ -2006,11 +1992,11 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Prdm16</t>
+          <t>Slc47a1</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.7</v>
+        <v>0.99</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
@@ -2021,11 +2007,11 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Lama3</t>
+          <t>Tbx15</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.51</v>
+        <v>0.61</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
@@ -2036,11 +2022,11 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Vegfc</t>
+          <t>Tspan11</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.73</v>
+        <v>0.85</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
@@ -2051,30 +2037,30 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Plcg2</t>
+          <t>Slc4a10</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.49</v>
+        <v>1</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>0.4</t>
+          <t>0.4, 0.5</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Arl15</t>
+          <t>Slc47a2</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.99</v>
+        <v>0.71</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>0.5</t>
+          <t>0.4, 0.5</t>
         </is>
       </c>
     </row>
@@ -2215,6 +2201,162 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:C9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Gene</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>pts</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>pts of origin</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Sema3g</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>0.36</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>0.3</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Bmx</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>0.3, 0.4, 0.5</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Nos1</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>0.36</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>0.3</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Prdm16</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>0.3, 0.4, 0.5</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Lama3</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>0.51</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>0.3, 0.4, 0.5</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Vegfc</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>0.73</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>0.4, 0.5</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Plcg2</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>0.49</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>0.4</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Pecam1</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>0.77</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>0.5</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2320,7 +2462,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2429,11 +2571,11 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Fndc1</t>
+          <t>Rspo2</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.6899999999999999</v>
+        <v>0.52</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
@@ -2444,11 +2586,11 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Rspo2</t>
+          <t>Fndc1</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.52</v>
+        <v>0.6899999999999999</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
@@ -2461,7 +2603,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2579,117 +2721,6 @@
       <c r="C7" t="inlineStr">
         <is>
           <t>0.5</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Gene</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>pts</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>pts of origin</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Mamdc2</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>0.53</v>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>0.3, 0.4, 0.5</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Abca8a</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>0.75</v>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>0.3, 0.4, 0.5</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Ror2</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>0.53</v>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>0.3, 0.4, 0.5</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Matn2</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>0.53</v>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>0.3, 0.4, 0.5</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Col15a1</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>0.53</v>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>0.3, 0.4, 0.5</t>
         </is>
       </c>
     </row>
@@ -2732,6 +2763,117 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
+          <t>Mamdc2</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>0.53</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>0.3, 0.4, 0.5</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Abca8a</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>0.3, 0.4, 0.5</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Ror2</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>0.53</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>0.3, 0.4, 0.5</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Matn2</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>0.53</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>0.3, 0.4, 0.5</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Vit</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>0.53</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>0.3, 0.4, 0.5</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Gene</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>pts</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>pts of origin</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
           <t>Col25a1</t>
         </is>
       </c>
@@ -2810,6 +2952,414 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Gene</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>pts</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>pts of origin</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>C6</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>0.34</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>0.3</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Kng2</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>0.51</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>0.3, 0.4, 0.5</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Ror2</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>0.68</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>0.3, 0.4, 0.5</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Col15a1</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>0.3, 0.4, 0.5</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Fap</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>0.57</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>0.3, 0.4, 0.5</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Runx1</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>0.62</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>0.4, 0.5</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Gene</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>pts</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>pts of origin</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Gna14</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>0.3, 0.4, 0.5</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Itgb4</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>0.51</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>0.3, 0.4, 0.5</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Ptch1</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>0.8100000000000001</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>0.3, 0.4, 0.5</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Ngf</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>0.43</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>0.3, 0.4</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Ebf2</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>0.86</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>0.3, 0.4, 0.5</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>9130410C08Rik</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>0.5600000000000001</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>0.5</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Gene</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>pts</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>pts of origin</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Slco1a4</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>0.68</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>0.3, 0.4, 0.5</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Slco1c1</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>0.32</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>0.3</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Spock2</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>0.3</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Adgrl4</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>0.53</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>0.3, 0.4, 0.5</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Tmtc2</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>0.72</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>0.3, 0.4, 0.5</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Lef1</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>0.46</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>0.4</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Mecom</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>0.62</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>0.4, 0.5</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Flt1</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>0.72</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>0.5</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2843,11 +3393,11 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Gna14</t>
+          <t>Trpm3</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.5</v>
+        <v>0.9399999999999999</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -2858,378 +3408,81 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Itgb4</t>
+          <t>Cntnap5b</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.51</v>
+        <v>0.36</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>0.3, 0.4, 0.5</t>
+          <t>0.3</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Ptch1</t>
+          <t>Gria3</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.8100000000000001</v>
+        <v>0.41</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>0.3, 0.4, 0.5</t>
+          <t>0.3, 0.4</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Ror2</t>
+          <t>Kirrel3</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.46</v>
+        <v>0.62</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>0.3, 0.4</t>
+          <t>0.3, 0.4, 0.5</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Ngf</t>
+          <t>Lsamp</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.43</v>
+        <v>0.95</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>0.3, 0.4</t>
+          <t>0.3, 0.4, 0.5</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Ebf2</t>
+          <t>Kcnip4</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.86</v>
+        <v>0.87</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>0.5</t>
+          <t>0.4, 0.5</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>9130410C08Rik</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
-        <v>0.5600000000000001</v>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>0.5</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Gene</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>pts</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>pts of origin</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Slco1a4</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>0.68</v>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>0.3, 0.4, 0.5</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Slco1c1</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>0.32</v>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>0.3</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Spock2</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>0.31</v>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>0.3</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Adgrl4</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>0.53</v>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>0.3, 0.4, 0.5</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Tmtc2</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>0.72</v>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>0.3, 0.4, 0.5</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Lef1</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>0.46</v>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>0.4</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Mecom</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
-        <v>0.62</v>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>0.4, 0.5</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>Flt1</t>
-        </is>
-      </c>
-      <c r="B9" t="n">
-        <v>0.72</v>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>0.5</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Gene</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>pts</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>pts of origin</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Trpm3</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>0.9399999999999999</v>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>0.3, 0.4, 0.5</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Cntnap5b</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>0.36</v>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>0.3</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Gria3</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>0.41</v>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>0.3, 0.4</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Kirrel3</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>0.62</v>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>0.3, 0.4, 0.5</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Lsamp</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>0.95</v>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>0.3, 0.4, 0.5</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Kcnip4</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>0.87</v>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>0.4, 0.5</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
           <t>Nrxn3</t>
         </is>
       </c>
@@ -3239,117 +3492,6 @@
       <c r="C8" t="inlineStr">
         <is>
           <t>0.5</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Gene</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>pts</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>pts of origin</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Sorbs2</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>0.6899999999999999</v>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>0.3, 0.4, 0.5</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Frmd5</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>0.78</v>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>0.3, 0.4, 0.5</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Ptprg</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>0.84</v>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>0.3, 0.4, 0.5</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Cmss1</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>0.78</v>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>0.3, 0.4, 0.5</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Gphn</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>0.9399999999999999</v>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>0.3, 0.4, 0.5</t>
         </is>
       </c>
     </row>
@@ -3392,11 +3534,11 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Myo1f</t>
+          <t>Sorbs2</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.57</v>
+        <v>0.6899999999999999</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -3407,11 +3549,11 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Runx1</t>
+          <t>Frmd5</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.61</v>
+        <v>0.78</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
@@ -3422,11 +3564,11 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Dock2</t>
+          <t>Ptprg</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.65</v>
+        <v>0.84</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
@@ -3437,11 +3579,11 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Lyn</t>
+          <t>Cmss1</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.74</v>
+        <v>0.78</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
@@ -3452,11 +3594,11 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Ppm1h</t>
+          <t>Gphn</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.83</v>
+        <v>0.9399999999999999</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
@@ -3470,6 +3612,117 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Gene</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>pts</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>pts of origin</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Myo1f</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>0.57</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>0.3, 0.4, 0.5</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Runx1</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>0.61</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>0.3, 0.4, 0.5</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Dock2</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>0.3, 0.4, 0.5</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Lyn</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>0.74</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>0.3, 0.4, 0.5</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Ppm1h</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>0.83</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>0.3, 0.4, 0.5</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -3608,175 +3861,4 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Gene</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>pts</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>pts of origin</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Slco1c1</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>0.68</v>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>0.3, 0.4, 0.5</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Slco1a4</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>0.95</v>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>0.3, 0.4, 0.5</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Slc7a5</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>0.44</v>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>0.3, 0.4</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Nostrin</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>0.41</v>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>0.3, 0.4</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Tfrc</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>0.37</v>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>0.3</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Prom1</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>0.43</v>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>0.4</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Spock2</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
-        <v>0.66</v>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>0.5</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>Lef1</t>
-        </is>
-      </c>
-      <c r="B9" t="n">
-        <v>0.86</v>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>0.5</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Slc39a10</t>
-        </is>
-      </c>
-      <c r="B10" t="n">
-        <v>0.7</v>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>0.5</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
 </file>
</xml_diff>